<commit_message>
Ajustada con bambios de unidades reportados por presidencia el viernes 11 de enero
</commit_message>
<xml_diff>
--- a/5.GestionDotaciones/DAPRE/AbuDhabi/Seguimiento.xlsx
+++ b/5.GestionDotaciones/DAPRE/AbuDhabi/Seguimiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea Ospina Patiño\Documents\GitHub\Dotaciones2019\5.GestionDotaciones\DAPRE\AbuDhabi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F644C31-1116-4E6D-875E-5B9461C9DFAB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4A5A2E-78E6-4785-9E51-1C0300948886}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="COSTOS" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SeguimientoUDSAbuDhabiDAPRE!$A$2:$L$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SeguimientoUDSAbuDhabiDAPRE!$A$2:$L$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
   <si>
     <t>SERVICIO</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Cundinamarca</t>
   </si>
   <si>
-    <t>Córdoba</t>
-  </si>
-  <si>
     <t>Dotación gestionada</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>Soacha</t>
   </si>
   <si>
-    <t>Magdalena</t>
-  </si>
-  <si>
     <t>Santander</t>
   </si>
   <si>
@@ -166,52 +160,10 @@
     <t>Cupos</t>
   </si>
   <si>
-    <t>Técnica Comercial La Inmaculada</t>
-  </si>
-  <si>
-    <t>Bohórquez</t>
-  </si>
-  <si>
-    <t>Campo De La Cruz</t>
-  </si>
-  <si>
-    <t>Puerto Libertador</t>
-  </si>
-  <si>
-    <t>Pablo VI</t>
-  </si>
-  <si>
-    <t>Cordoba</t>
-  </si>
-  <si>
-    <t>San Bernardo del Viento</t>
-  </si>
-  <si>
-    <t>CDI San Bernardo del Viento</t>
-  </si>
-  <si>
     <t>Pacho</t>
   </si>
   <si>
     <t>Nuevo Amanecer</t>
-  </si>
-  <si>
-    <t>El Banco</t>
-  </si>
-  <si>
-    <t>IE Anaxímedes Torres- antiguo Julián Mejía Alvarado</t>
-  </si>
-  <si>
-    <t>Fondo de adaptación</t>
-  </si>
-  <si>
-    <t>Campo de la Cruz I</t>
-  </si>
-  <si>
-    <t>Campo de la Cruz II</t>
-  </si>
-  <si>
-    <t>Campo de la Cruz III</t>
   </si>
   <si>
     <t>Dotación parcial</t>
@@ -233,20 +185,6 @@
 Desde el Equipo de Dotación se envió a la Regional el Listado de mínimos de dotación requeridos para confirmar disponibilidad de recursos con el Ente Territorial.
 Ver adjuntos: TrazabilidadDotacionValleOrtigal-Cauca.pdf y MínimosDotacion_ValleOrtigalCauca.pdf
 En el marco del Convenio 007  de 2016 se ha presentado la  necesidad de dotación de esta infraestructura. Se espera la Prorroga al Convenio para recibir los recursos del Fondo Abu Dhabi para la compra de las dotaciones.</t>
-  </si>
-  <si>
-    <t>La Regional  ICBF no manifiesta  gestión con Entes territoriales para la adquisición de la Dotación.
-Desde el Equipo de Dotación se envió a la Regional el Listado de mínimos de dotación requeridos para confirmar disponibilidad de recursos con el Ente Territorial.
-Ver adjuntos: TrazabilidadDotacionPabloVI_Cordoba.pdf y MínimosDotacionPabloVI_Cordoba.pdf
-En el marco del Convenio 007  de 2016 se ha presentado la  necesidad de dotación de esta infraestructura. Se espera la Prorroga al Convenio para recibir los recursos del Fondo Abu Dhabi para la compra de las dotaciones.</t>
-  </si>
-  <si>
-    <t>TrazabilidadDotacionSanBernardo_Cordoba.pdf</t>
-  </si>
-  <si>
-    <t>En acta de reunión con la Alcaldía de San Bernardo de Viento (9 mayo 2018), quedó como compromiso por parte de la Alcaldía remitir propuesta sobre la compra dotación inicial de acuerdo a los recursos disponibles para la puesta en operación del CDI. No se ha obtenido respuesta de la alcaldía.
-Ver adjunto: TrazabilidadDotacionSanBernardo_Cordoba.pdf
-En el marco del Convenio 007  de 2016 se ha presentado la  necesidad de dotacipon de esta infraestructura. Se espera la Prorroga al Convenio para recibir los recursos del Fondo Abu Dhabi para la compra de las dotaciones.</t>
   </si>
   <si>
     <t>Dotación Parcial</t>
@@ -322,22 +260,6 @@
     </r>
   </si>
   <si>
-    <t>La Regional  ICBF no manifiesta  gestión con Entes territoriales para la adquisición de la Dotación. Desde el Equipo de Dotación se están gestionado los Listados mínimos de dotación requeridos.
-Ver adjunto: TrazabilidadDotacion_CampoCruzAtlantico.pdf
-En el marco del Convenio 007  de 2016 se ha presentado la  necesidad de dotación de esta infraestructura. Se espera la Prorroga al Convenio para recibir los recursos del Fondo Abu Dhabi para la compra de las dotaciones.</t>
-  </si>
-  <si>
-    <t>La Regional  ICBF no manifiesta  gestión con Entes territoriales para la adquisición de la Dotación. Desde el Equipo de Dotación se están gestionado los Listados mínimos de dotación requeridos.
-Ver adjunto: TrazabilidadDotacion_ElBancoMagdalena.pdf
-En el marco del Convenio 007  de 2016 se ha presentado la  necesidad de dotación de esta infraestructura. Se espera la Prorroga al Convenio para recibir los recursos del Fondo Abu Dhabi para la compra de las dotaciones.</t>
-  </si>
-  <si>
-    <t>TrazabilidadDotacion_ElBancoMagdalena.pdf</t>
-  </si>
-  <si>
-    <t>TrazabilidadDotacion_CampoCruzAtlantico.pdf</t>
-  </si>
-  <si>
     <t>La Alcaldía manifestó mediante oficio de respuesta a la solicitud de la Subdirección de Operación de la Dirección de Primera Infancia, que invertiría recursos CONPES en la adquisición de la dotación completa para este CDI y desde el mes de septiembre de 2018, el Equipo de dotaciones ha realizado la articulación de la Regional con la Alcaldía para la compra de la dotación.
 Ver adjuntos: RespuestaCONPES_ÑaeMecheAmazonas. Pdf y TrazabilidadGestionDotacion_ÑaeMecheAmazonas.pdf</t>
   </si>
@@ -348,9 +270,6 @@
     <t>TrazabilidadDotacionValleOrtigal-Cauca.pdf y MínimosDotacion_ValleOrtigalCauca.pdf</t>
   </si>
   <si>
-    <t>TrazabilidadDotacionPabloVI_Cordoba.pdf y MínimosDotacionPabloVI_Cordoba.pdf</t>
-  </si>
-  <si>
     <t>Trazabilidad_NuevoAmanecerCundinamarca.pdf, MinimosDotacion_NuevoAmanecerCundinamarca.pdf y DotacionPendiente_NuevoAmanecerCundinamarca.xls</t>
   </si>
   <si>
@@ -358,6 +277,27 @@
   </si>
   <si>
     <t>ActaCampoMadrid_6Junio2018.pdf, MinimosDotacion_CampoMadridSantander.pdf y  TrazabilidadDotacion_CampoMadridSantander.pdf</t>
+  </si>
+  <si>
+    <t>Vida Nueva</t>
+  </si>
+  <si>
+    <t>La Inmaculada</t>
+  </si>
+  <si>
+    <t>Cúcuta</t>
+  </si>
+  <si>
+    <t>Cormoranes</t>
+  </si>
+  <si>
+    <t>Barranquilla</t>
+  </si>
+  <si>
+    <t>Las Gardenias</t>
+  </si>
+  <si>
+    <t>Norte de Santander</t>
   </si>
 </sst>
 </file>
@@ -371,7 +311,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="[$$-240A]\ #,##0;\-[$$-240A]\ #,##0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,18 +380,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="20"/>
       <color theme="1"/>
@@ -467,7 +395,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,24 +410,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC66FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF66FFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -544,19 +460,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -564,7 +467,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -602,40 +505,25 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -960,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="66" zoomScaleNormal="66" zoomScaleSheetLayoutView="148" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="148" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,32 +867,32 @@
     <col min="9" max="9" width="22.28515625" style="12" customWidth="1"/>
     <col min="10" max="10" width="55.5703125" style="12" customWidth="1"/>
     <col min="11" max="11" width="97.5703125" style="8" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="60.28515625" style="8" customWidth="1"/>
     <col min="13" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="27" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
+    <row r="1" spans="1:12" s="23" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
     </row>
     <row r="2" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>13</v>
@@ -1016,428 +904,323 @@
         <v>14</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>15</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="16" customFormat="1" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="17">
+        <v>65</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="20"/>
+    </row>
+    <row r="4" spans="1:12" ht="270.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="17">
+        <v>300</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="20"/>
+    </row>
+    <row r="5" spans="1:12" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="17">
+        <v>160</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="20"/>
+    </row>
+    <row r="6" spans="1:12" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="17">
+        <v>300</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" s="20"/>
+    </row>
+    <row r="7" spans="1:12" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="17">
+        <v>300</v>
+      </c>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="20"/>
+    </row>
+    <row r="8" spans="1:12" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="20"/>
+    </row>
+    <row r="9" spans="1:12" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="21">
+      <c r="F9" s="21"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="20"/>
+    </row>
+    <row r="10" spans="1:12" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="L3" s="18"/>
-    </row>
-    <row r="4" spans="1:12" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>4</v>
-      </c>
-      <c r="B4" s="21" t="s">
+      <c r="D10" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="21">
-        <v>60</v>
-      </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="K4" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="L4" s="24"/>
-    </row>
-    <row r="5" spans="1:12" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
-        <v>5</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="21">
-        <v>60</v>
-      </c>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="K5" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="L5" s="24"/>
-    </row>
-    <row r="6" spans="1:12" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
-        <v>6</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="21">
-        <v>60</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="K6" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="L6" s="24"/>
-    </row>
-    <row r="7" spans="1:12" ht="270.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>8</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="21">
-        <v>300</v>
-      </c>
-      <c r="H7" s="23" t="s">
+      <c r="E10" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="20"/>
+    </row>
+    <row r="11" spans="1:12" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="K7" s="22" t="s">
+      <c r="D11" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L7" s="17"/>
-    </row>
-    <row r="8" spans="1:12" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>7</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="21">
-        <v>60</v>
-      </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="K8" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="L8" s="24"/>
-    </row>
-    <row r="9" spans="1:12" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
-        <v>9</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="21">
-        <v>95</v>
-      </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="K9" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="L9" s="24"/>
-    </row>
-    <row r="10" spans="1:12" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="F11" s="21"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="20"/>
+    </row>
+    <row r="12" spans="1:12" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
         <v>10</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="21">
-        <v>160</v>
-      </c>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="K10" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="L10" s="24"/>
-    </row>
-    <row r="11" spans="1:12" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
-        <v>3</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="21">
-        <v>300</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="J11" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="K11" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="L11" s="17"/>
-    </row>
-    <row r="12" spans="1:12" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
-        <v>2</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="21">
-        <v>300</v>
-      </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="L12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="20"/>
     </row>
     <row r="13" spans="1:12" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>11</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="21">
-        <v>60</v>
-      </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="L13" s="24"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="19"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="K14"/>
-    </row>
-    <row r="15" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="K15"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K16" s="7"/>
-    </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K17" s="7"/>
-    </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K18" s="7"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:L13" xr:uid="{84089222-54C1-4B0E-8D21-2D624704F814}"/>
+  <autoFilter ref="A2:L8" xr:uid="{84089222-54C1-4B0E-8D21-2D624704F814}"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="93" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>